<commit_message>
Added abstract to the paper draft
</commit_message>
<xml_diff>
--- a/excel_files/US.xlsx
+++ b/excel_files/US.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="US" sheetId="1" state="visible" r:id="rId1"/>
@@ -54,18 +54,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D124"/>
+  <dimension ref="A1:E111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -387,6 +387,11 @@
           <t>weekday</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Increase in Cases</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -405,141 +410,165 @@
           <t>Tuesday</t>
         </is>
       </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2020-01-22</t>
+          <t>2020-01-24</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Wednesday</t>
-        </is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2020-01-23</t>
+          <t>2020-01-25</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Thursday</t>
-        </is>
+          <t>Saturday</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2020-01-24</t>
+          <t>2020-01-26</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Friday</t>
-        </is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2020-01-25</t>
+          <t>2020-01-30</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Saturday</t>
-        </is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2020-01-26</t>
+          <t>2020-01-31</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Sunday</t>
-        </is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2020-01-27</t>
+          <t>2020-02-01</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Monday</t>
-        </is>
+          <t>Saturday</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2020-01-28</t>
+          <t>2020-02-02</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Tuesday</t>
-        </is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2020-01-29</t>
+          <t>2020-02-05</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
@@ -549,2060 +578,2132 @@
           <t>Wednesday</t>
         </is>
       </c>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2020-01-30</t>
+          <t>2020-02-10</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Thursday</t>
-        </is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2020-01-31</t>
+          <t>2020-02-12</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Friday</t>
-        </is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2020-02-01</t>
+          <t>2020-02-13</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Saturday</t>
-        </is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2020-02-02</t>
+          <t>2020-02-17</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Sunday</t>
-        </is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2020-02-03</t>
+          <t>2020-02-20</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Monday</t>
-        </is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2020-02-04</t>
+          <t>2020-02-21</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Tuesday</t>
-        </is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2020-02-05</t>
+          <t>2020-02-24</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Wednesday</t>
-        </is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2020-02-06</t>
+          <t>2020-02-25</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Thursday</t>
-        </is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2020-02-07</t>
+          <t>2020-02-26</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Friday</t>
-        </is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2020-02-08</t>
+          <t>2020-02-28</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Saturday</t>
-        </is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2020-02-09</t>
+          <t>2020-02-29</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Sunday</t>
-        </is>
+          <t>Saturday</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2020-02-10</t>
+          <t>2020-03-01</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>13</v>
+        <v>88</v>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Monday</t>
-        </is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2020-02-11</t>
+          <t>2020-03-02</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>13</v>
+        <v>104</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Tuesday</t>
-        </is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2020-02-12</t>
+          <t>2020-03-03</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>14</v>
+        <v>125</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Wednesday</t>
-        </is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2020-02-13</t>
+          <t>2020-03-04</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>15</v>
+        <v>161</v>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Thursday</t>
-        </is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>36</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-03-05</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>15</v>
+        <v>228</v>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Friday</t>
-        </is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>67</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2020-02-15</t>
+          <t>2020-03-06</t>
         </is>
       </c>
       <c r="B27" t="n">
+        <v>311</v>
+      </c>
+      <c r="C27" t="n">
         <v>15</v>
       </c>
-      <c r="C27" t="n">
-        <v>0</v>
-      </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Saturday</t>
-        </is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>83</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2020-02-16</t>
+          <t>2020-03-07</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>15</v>
+        <v>428</v>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Sunday</t>
-        </is>
+          <t>Saturday</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>117</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2020-02-17</t>
+          <t>2020-03-08</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>25</v>
+        <v>547</v>
       </c>
       <c r="C29" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Monday</t>
-        </is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>119</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2020-02-18</t>
+          <t>2020-03-09</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>25</v>
+        <v>748</v>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Tuesday</t>
-        </is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>201</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2020-02-19</t>
+          <t>2020-03-10</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>25</v>
+        <v>1018</v>
       </c>
       <c r="C31" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Wednesday</t>
-        </is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>270</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2020-02-20</t>
+          <t>2020-03-11</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>27</v>
+        <v>1263</v>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Thursday</t>
-        </is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>245</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2020-02-21</t>
+          <t>2020-03-12</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>30</v>
+        <v>1668</v>
       </c>
       <c r="C33" t="n">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Friday</t>
-        </is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>405</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2020-02-22</t>
+          <t>2020-03-13</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>30</v>
+        <v>2224</v>
       </c>
       <c r="C34" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Saturday</t>
-        </is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>556</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2020-02-23</t>
+          <t>2020-03-14</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>30</v>
+        <v>2898</v>
       </c>
       <c r="C35" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Sunday</t>
-        </is>
+          <t>Saturday</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>674</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2020-02-24</t>
+          <t>2020-03-15</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>43</v>
+        <v>3600</v>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Monday</t>
-        </is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>702</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2020-02-25</t>
+          <t>2020-03-16</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>45</v>
+        <v>4507</v>
       </c>
       <c r="C37" t="n">
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Tuesday</t>
-        </is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>907</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2020-02-26</t>
+          <t>2020-03-17</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>60</v>
+        <v>5906</v>
       </c>
       <c r="C38" t="n">
-        <v>0</v>
+        <v>117</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Wednesday</t>
-        </is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>1399</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2020-02-27</t>
+          <t>2020-03-18</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>60</v>
+        <v>8350</v>
       </c>
       <c r="C39" t="n">
-        <v>0</v>
+        <v>162</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Thursday</t>
-        </is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>2444</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2020-02-28</t>
+          <t>2020-03-19</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>65</v>
+        <v>12393</v>
       </c>
       <c r="C40" t="n">
-        <v>0</v>
+        <v>212</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Friday</t>
-        </is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>4043</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2020-02-29</t>
+          <t>2020-03-20</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>70</v>
+        <v>18001</v>
       </c>
       <c r="C41" t="n">
-        <v>1</v>
+        <v>275</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Saturday</t>
-        </is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>5608</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2020-03-01</t>
+          <t>2020-03-21</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>88</v>
+        <v>24526</v>
       </c>
       <c r="C42" t="n">
-        <v>3</v>
+        <v>358</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Sunday</t>
-        </is>
+          <t>Saturday</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>6525</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2020-03-02</t>
+          <t>2020-03-22</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>104</v>
+        <v>33063</v>
       </c>
       <c r="C43" t="n">
-        <v>6</v>
+        <v>455</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Monday</t>
-        </is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>8537</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2020-03-03</t>
+          <t>2020-03-23</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>125</v>
+        <v>43500</v>
       </c>
       <c r="C44" t="n">
-        <v>10</v>
+        <v>574</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Tuesday</t>
-        </is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>10437</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2020-03-04</t>
+          <t>2020-03-24</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>161</v>
+        <v>53924</v>
       </c>
       <c r="C45" t="n">
-        <v>12</v>
+        <v>769</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Wednesday</t>
-        </is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>10424</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2020-03-05</t>
+          <t>2020-03-25</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>228</v>
+        <v>68530</v>
       </c>
       <c r="C46" t="n">
-        <v>12</v>
+        <v>1039</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Thursday</t>
-        </is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>14606</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2020-03-06</t>
+          <t>2020-03-26</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>311</v>
+        <v>85558</v>
       </c>
       <c r="C47" t="n">
-        <v>15</v>
+        <v>1345</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Friday</t>
-        </is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>17028</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2020-03-07</t>
+          <t>2020-03-27</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>428</v>
+        <v>102829</v>
       </c>
       <c r="C48" t="n">
-        <v>19</v>
+        <v>1758</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Saturday</t>
-        </is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>17271</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2020-03-08</t>
+          <t>2020-03-28</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>547</v>
+        <v>123723</v>
       </c>
       <c r="C49" t="n">
-        <v>22</v>
+        <v>2287</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Sunday</t>
-        </is>
+          <t>Saturday</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>20894</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2020-03-09</t>
+          <t>2020-03-29</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>748</v>
+        <v>142397</v>
       </c>
       <c r="C50" t="n">
-        <v>26</v>
+        <v>2702</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Monday</t>
-        </is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>18674</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2020-03-10</t>
+          <t>2020-03-30</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>1018</v>
+        <v>163863</v>
       </c>
       <c r="C51" t="n">
-        <v>31</v>
+        <v>3356</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Tuesday</t>
-        </is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="E51" t="n">
+        <v>21466</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2020-03-11</t>
+          <t>2020-03-31</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>1263</v>
+        <v>188413</v>
       </c>
       <c r="C52" t="n">
-        <v>37</v>
+        <v>4290</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Wednesday</t>
-        </is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="E52" t="n">
+        <v>24550</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2020-03-12</t>
+          <t>2020-04-01</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>1668</v>
+        <v>215161</v>
       </c>
       <c r="C53" t="n">
-        <v>43</v>
+        <v>5315</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Thursday</t>
-        </is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
+        <v>26748</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2020-03-13</t>
+          <t>2020-04-02</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>2224</v>
+        <v>244619</v>
       </c>
       <c r="C54" t="n">
-        <v>50</v>
+        <v>6542</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Friday</t>
-        </is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>29458</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2020-03-14</t>
+          <t>2020-04-03</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>2898</v>
+        <v>277262</v>
       </c>
       <c r="C55" t="n">
-        <v>60</v>
+        <v>7902</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Saturday</t>
-        </is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
+        <v>32643</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2020-03-15</t>
+          <t>2020-04-04</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>3600</v>
+        <v>312498</v>
       </c>
       <c r="C56" t="n">
-        <v>68</v>
+        <v>9466</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Sunday</t>
-        </is>
+          <t>Saturday</t>
+        </is>
+      </c>
+      <c r="E56" t="n">
+        <v>35236</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2020-03-16</t>
+          <t>2020-04-05</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>4507</v>
+        <v>337959</v>
       </c>
       <c r="C57" t="n">
-        <v>91</v>
+        <v>10828</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Monday</t>
-        </is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="E57" t="n">
+        <v>25461</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2020-03-17</t>
+          <t>2020-04-06</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>5906</v>
+        <v>367568</v>
       </c>
       <c r="C58" t="n">
-        <v>117</v>
+        <v>12330</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Tuesday</t>
-        </is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="E58" t="n">
+        <v>29609</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2020-03-18</t>
+          <t>2020-04-07</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>8350</v>
+        <v>399352</v>
       </c>
       <c r="C59" t="n">
-        <v>162</v>
+        <v>14579</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Wednesday</t>
-        </is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="E59" t="n">
+        <v>31784</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2020-03-19</t>
+          <t>2020-04-08</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>12393</v>
+        <v>431169</v>
       </c>
       <c r="C60" t="n">
-        <v>212</v>
+        <v>16673</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Thursday</t>
-        </is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="E60" t="n">
+        <v>31817</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2020-03-20</t>
+          <t>2020-04-09</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>18001</v>
+        <v>465859</v>
       </c>
       <c r="C61" t="n">
-        <v>275</v>
+        <v>18772</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Friday</t>
-        </is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="E61" t="n">
+        <v>34690</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2020-03-21</t>
+          <t>2020-04-10</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>24526</v>
+        <v>499325</v>
       </c>
       <c r="C62" t="n">
-        <v>358</v>
+        <v>21028</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Saturday</t>
-        </is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="E62" t="n">
+        <v>33466</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2020-03-22</t>
+          <t>2020-04-11</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>33063</v>
+        <v>531042</v>
       </c>
       <c r="C63" t="n">
-        <v>455</v>
+        <v>23105</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Sunday</t>
-        </is>
+          <t>Saturday</t>
+        </is>
+      </c>
+      <c r="E63" t="n">
+        <v>31717</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2020-03-23</t>
+          <t>2020-04-12</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>43500</v>
+        <v>558182</v>
       </c>
       <c r="C64" t="n">
-        <v>574</v>
+        <v>24785</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Monday</t>
-        </is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="E64" t="n">
+        <v>27140</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2020-03-24</t>
+          <t>2020-04-13</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>53924</v>
+        <v>583940</v>
       </c>
       <c r="C65" t="n">
-        <v>769</v>
+        <v>26547</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Tuesday</t>
-        </is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="E65" t="n">
+        <v>25758</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2020-03-25</t>
+          <t>2020-04-14</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>68530</v>
+        <v>610615</v>
       </c>
       <c r="C66" t="n">
-        <v>1039</v>
+        <v>29246</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Wednesday</t>
-        </is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="E66" t="n">
+        <v>26675</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2020-03-26</t>
+          <t>2020-04-15</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>85558</v>
+        <v>640637</v>
       </c>
       <c r="C67" t="n">
-        <v>1345</v>
+        <v>31994</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Thursday</t>
-        </is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="E67" t="n">
+        <v>30022</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2020-03-27</t>
+          <t>2020-04-16</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>102829</v>
+        <v>672243</v>
       </c>
       <c r="C68" t="n">
-        <v>1758</v>
+        <v>34264</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Friday</t>
-        </is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="E68" t="n">
+        <v>31606</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2020-03-28</t>
+          <t>2020-04-17</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>123723</v>
+        <v>703740</v>
       </c>
       <c r="C69" t="n">
-        <v>2287</v>
+        <v>36626</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Saturday</t>
-        </is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="E69" t="n">
+        <v>31497</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2020-03-29</t>
+          <t>2020-04-18</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>142397</v>
+        <v>732121</v>
       </c>
       <c r="C70" t="n">
-        <v>2702</v>
+        <v>38571</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Sunday</t>
-        </is>
+          <t>Saturday</t>
+        </is>
+      </c>
+      <c r="E70" t="n">
+        <v>28381</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2020-03-30</t>
+          <t>2020-04-19</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>163863</v>
+        <v>757475</v>
       </c>
       <c r="C71" t="n">
-        <v>3356</v>
+        <v>40089</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Monday</t>
-        </is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="E71" t="n">
+        <v>25354</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2020-03-31</t>
+          <t>2020-04-20</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>188413</v>
+        <v>784761</v>
       </c>
       <c r="C72" t="n">
-        <v>4290</v>
+        <v>41919</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Tuesday</t>
-        </is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="E72" t="n">
+        <v>27286</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2020-04-01</t>
+          <t>2020-04-21</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>215161</v>
+        <v>810249</v>
       </c>
       <c r="C73" t="n">
-        <v>5315</v>
+        <v>44587</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Wednesday</t>
-        </is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="E73" t="n">
+        <v>25488</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2020-04-02</t>
+          <t>2020-04-22</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>244619</v>
+        <v>839017</v>
       </c>
       <c r="C74" t="n">
-        <v>6542</v>
+        <v>46955</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Thursday</t>
-        </is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="E74" t="n">
+        <v>28768</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2020-04-03</t>
+          <t>2020-04-23</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>277262</v>
+        <v>872805</v>
       </c>
       <c r="C75" t="n">
-        <v>7902</v>
+        <v>49123</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Friday</t>
-        </is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="E75" t="n">
+        <v>33788</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2020-04-04</t>
+          <t>2020-04-24</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>312498</v>
+        <v>909530</v>
       </c>
       <c r="C76" t="n">
-        <v>9466</v>
+        <v>51250</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Saturday</t>
-        </is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="E76" t="n">
+        <v>36725</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2020-04-05</t>
+          <t>2020-04-25</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>337959</v>
+        <v>943802</v>
       </c>
       <c r="C77" t="n">
-        <v>10828</v>
+        <v>53210</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Sunday</t>
-        </is>
+          <t>Saturday</t>
+        </is>
+      </c>
+      <c r="E77" t="n">
+        <v>34272</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2020-04-06</t>
+          <t>2020-04-26</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>367568</v>
+        <v>970409</v>
       </c>
       <c r="C78" t="n">
-        <v>12330</v>
+        <v>54465</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Monday</t>
-        </is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="E78" t="n">
+        <v>26607</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2020-04-07</t>
+          <t>2020-04-27</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>399352</v>
+        <v>993747</v>
       </c>
       <c r="C79" t="n">
-        <v>14579</v>
+        <v>56022</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Tuesday</t>
-        </is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="E79" t="n">
+        <v>23338</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2020-04-08</t>
+          <t>2020-04-28</t>
         </is>
       </c>
       <c r="B80" t="n">
-        <v>431169</v>
+        <v>1018399</v>
       </c>
       <c r="C80" t="n">
-        <v>16673</v>
+        <v>58416</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Wednesday</t>
-        </is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="E80" t="n">
+        <v>24652</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2020-04-09</t>
+          <t>2020-04-29</t>
         </is>
       </c>
       <c r="B81" t="n">
-        <v>465859</v>
+        <v>1045102</v>
       </c>
       <c r="C81" t="n">
-        <v>18772</v>
+        <v>60930</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Thursday</t>
-        </is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="E81" t="n">
+        <v>26703</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2020-04-10</t>
+          <t>2020-04-30</t>
         </is>
       </c>
       <c r="B82" t="n">
-        <v>499325</v>
+        <v>1075517</v>
       </c>
       <c r="C82" t="n">
-        <v>21028</v>
+        <v>63140</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Friday</t>
-        </is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="E82" t="n">
+        <v>30415</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2020-04-11</t>
+          <t>2020-05-01</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>531042</v>
+        <v>1109476</v>
       </c>
       <c r="C83" t="n">
-        <v>23105</v>
+        <v>64902</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Saturday</t>
-        </is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="E83" t="n">
+        <v>33959</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>2020-04-12</t>
+          <t>2020-05-02</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>558182</v>
+        <v>1138944</v>
       </c>
       <c r="C84" t="n">
-        <v>24785</v>
+        <v>66485</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Sunday</t>
-        </is>
+          <t>Saturday</t>
+        </is>
+      </c>
+      <c r="E84" t="n">
+        <v>29468</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2020-04-13</t>
+          <t>2020-05-03</t>
         </is>
       </c>
       <c r="B85" t="n">
-        <v>583940</v>
+        <v>1165013</v>
       </c>
       <c r="C85" t="n">
-        <v>26547</v>
+        <v>67816</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Monday</t>
-        </is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="E85" t="n">
+        <v>26069</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>2020-04-14</t>
+          <t>2020-05-04</t>
         </is>
       </c>
       <c r="B86" t="n">
-        <v>610615</v>
+        <v>1186965</v>
       </c>
       <c r="C86" t="n">
-        <v>29246</v>
+        <v>68905</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Tuesday</t>
-        </is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="E86" t="n">
+        <v>21952</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>2020-04-15</t>
+          <t>2020-05-05</t>
         </is>
       </c>
       <c r="B87" t="n">
-        <v>640637</v>
+        <v>1210669</v>
       </c>
       <c r="C87" t="n">
-        <v>31994</v>
+        <v>71139</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Wednesday</t>
-        </is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="E87" t="n">
+        <v>23704</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>2020-04-16</t>
+          <t>2020-05-06</t>
         </is>
       </c>
       <c r="B88" t="n">
-        <v>672243</v>
+        <v>1235174</v>
       </c>
       <c r="C88" t="n">
-        <v>34264</v>
+        <v>73847</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Thursday</t>
-        </is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="E88" t="n">
+        <v>24505</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>2020-04-17</t>
+          <t>2020-05-07</t>
         </is>
       </c>
       <c r="B89" t="n">
-        <v>703740</v>
+        <v>1263668</v>
       </c>
       <c r="C89" t="n">
-        <v>36626</v>
+        <v>75805</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Friday</t>
-        </is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="E89" t="n">
+        <v>28494</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>2020-04-18</t>
+          <t>2020-05-08</t>
         </is>
       </c>
       <c r="B90" t="n">
-        <v>732121</v>
+        <v>1291329</v>
       </c>
       <c r="C90" t="n">
-        <v>38571</v>
+        <v>77380</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Saturday</t>
-        </is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="E90" t="n">
+        <v>27661</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>2020-04-19</t>
+          <t>2020-05-09</t>
         </is>
       </c>
       <c r="B91" t="n">
-        <v>757475</v>
+        <v>1316167</v>
       </c>
       <c r="C91" t="n">
-        <v>40089</v>
+        <v>78834</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Sunday</t>
-        </is>
+          <t>Saturday</t>
+        </is>
+      </c>
+      <c r="E91" t="n">
+        <v>24838</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>2020-04-20</t>
+          <t>2020-05-10</t>
         </is>
       </c>
       <c r="B92" t="n">
-        <v>784761</v>
+        <v>1336478</v>
       </c>
       <c r="C92" t="n">
-        <v>41919</v>
+        <v>79765</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Monday</t>
-        </is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="E92" t="n">
+        <v>20311</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>2020-04-21</t>
+          <t>2020-05-11</t>
         </is>
       </c>
       <c r="B93" t="n">
-        <v>810249</v>
+        <v>1354096</v>
       </c>
       <c r="C93" t="n">
-        <v>44587</v>
+        <v>80747</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Tuesday</t>
-        </is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="E93" t="n">
+        <v>17618</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>2020-04-22</t>
+          <t>2020-05-12</t>
         </is>
       </c>
       <c r="B94" t="n">
-        <v>839017</v>
+        <v>1376388</v>
       </c>
       <c r="C94" t="n">
-        <v>46955</v>
+        <v>82400</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Wednesday</t>
-        </is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="E94" t="n">
+        <v>22292</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>2020-04-23</t>
+          <t>2020-05-13</t>
         </is>
       </c>
       <c r="B95" t="n">
-        <v>872805</v>
+        <v>1397520</v>
       </c>
       <c r="C95" t="n">
-        <v>49123</v>
+        <v>84168</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Thursday</t>
-        </is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="E95" t="n">
+        <v>21132</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>2020-04-24</t>
+          <t>2020-05-14</t>
         </is>
       </c>
       <c r="B96" t="n">
-        <v>909530</v>
+        <v>1424474</v>
       </c>
       <c r="C96" t="n">
-        <v>51250</v>
+        <v>85906</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Friday</t>
-        </is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="E96" t="n">
+        <v>26954</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>2020-04-25</t>
+          <t>2020-05-15</t>
         </is>
       </c>
       <c r="B97" t="n">
-        <v>943802</v>
+        <v>1450700</v>
       </c>
       <c r="C97" t="n">
-        <v>53210</v>
+        <v>87499</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Saturday</t>
-        </is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="E97" t="n">
+        <v>26226</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>2020-04-26</t>
+          <t>2020-05-16</t>
         </is>
       </c>
       <c r="B98" t="n">
-        <v>970409</v>
+        <v>1474351</v>
       </c>
       <c r="C98" t="n">
-        <v>54465</v>
+        <v>88724</v>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Sunday</t>
-        </is>
+          <t>Saturday</t>
+        </is>
+      </c>
+      <c r="E98" t="n">
+        <v>23651</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>2020-04-27</t>
+          <t>2020-05-17</t>
         </is>
       </c>
       <c r="B99" t="n">
-        <v>993747</v>
+        <v>1493350</v>
       </c>
       <c r="C99" t="n">
-        <v>56022</v>
+        <v>89568</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Monday</t>
-        </is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="E99" t="n">
+        <v>18999</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>2020-04-28</t>
+          <t>2020-05-18</t>
         </is>
       </c>
       <c r="B100" t="n">
-        <v>1018399</v>
+        <v>1515177</v>
       </c>
       <c r="C100" t="n">
-        <v>58416</v>
+        <v>90414</v>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Tuesday</t>
-        </is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="E100" t="n">
+        <v>21827</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>2020-04-29</t>
+          <t>2020-05-19</t>
         </is>
       </c>
       <c r="B101" t="n">
-        <v>1045102</v>
+        <v>1536129</v>
       </c>
       <c r="C101" t="n">
-        <v>60930</v>
+        <v>91934</v>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Wednesday</t>
-        </is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="E101" t="n">
+        <v>20952</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>2020-04-30</t>
+          <t>2020-05-20</t>
         </is>
       </c>
       <c r="B102" t="n">
-        <v>1075517</v>
+        <v>1559003</v>
       </c>
       <c r="C102" t="n">
-        <v>63140</v>
+        <v>93406</v>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Thursday</t>
-        </is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="E102" t="n">
+        <v>22874</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>2020-05-01</t>
+          <t>2020-05-21</t>
         </is>
       </c>
       <c r="B103" t="n">
-        <v>1109476</v>
+        <v>1584826</v>
       </c>
       <c r="C103" t="n">
-        <v>64902</v>
+        <v>94721</v>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Friday</t>
-        </is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="E103" t="n">
+        <v>25823</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>2020-05-02</t>
+          <t>2020-05-22</t>
         </is>
       </c>
       <c r="B104" t="n">
-        <v>1138944</v>
+        <v>1608710</v>
       </c>
       <c r="C104" t="n">
-        <v>66485</v>
+        <v>96010</v>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Saturday</t>
-        </is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="E104" t="n">
+        <v>23884</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>2020-05-03</t>
+          <t>2020-05-23</t>
         </is>
       </c>
       <c r="B105" t="n">
-        <v>1165013</v>
+        <v>1630912</v>
       </c>
       <c r="C105" t="n">
-        <v>67816</v>
+        <v>97060</v>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Sunday</t>
-        </is>
+          <t>Saturday</t>
+        </is>
+      </c>
+      <c r="E105" t="n">
+        <v>22202</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>2020-05-04</t>
+          <t>2020-05-24</t>
         </is>
       </c>
       <c r="B106" t="n">
-        <v>1186965</v>
+        <v>1651004</v>
       </c>
       <c r="C106" t="n">
-        <v>68905</v>
+        <v>97680</v>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Monday</t>
-        </is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="E106" t="n">
+        <v>20092</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>2020-05-05</t>
+          <t>2020-05-25</t>
         </is>
       </c>
       <c r="B107" t="n">
-        <v>1210669</v>
+        <v>1670101</v>
       </c>
       <c r="C107" t="n">
-        <v>71139</v>
+        <v>98190</v>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>Tuesday</t>
-        </is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="E107" t="n">
+        <v>19097</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>2020-05-06</t>
+          <t>2020-05-26</t>
         </is>
       </c>
       <c r="B108" t="n">
-        <v>1235174</v>
+        <v>1688990</v>
       </c>
       <c r="C108" t="n">
-        <v>73847</v>
+        <v>98937</v>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Wednesday</t>
-        </is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="E108" t="n">
+        <v>18889</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>2020-05-07</t>
+          <t>2020-05-27</t>
         </is>
       </c>
       <c r="B109" t="n">
-        <v>1263668</v>
+        <v>1707699</v>
       </c>
       <c r="C109" t="n">
-        <v>75805</v>
+        <v>100422</v>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>Thursday</t>
-        </is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="E109" t="n">
+        <v>18709</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>2020-05-08</t>
+          <t>2020-05-28</t>
         </is>
       </c>
       <c r="B110" t="n">
-        <v>1291329</v>
+        <v>1730158</v>
       </c>
       <c r="C110" t="n">
-        <v>77380</v>
+        <v>101622</v>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>Friday</t>
-        </is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="E110" t="n">
+        <v>22459</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>2020-05-09</t>
+          <t>2020-05-29</t>
         </is>
       </c>
       <c r="B111" t="n">
-        <v>1316167</v>
+        <v>1754724</v>
       </c>
       <c r="C111" t="n">
-        <v>78834</v>
+        <v>102812</v>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>Saturday</t>
-        </is>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="inlineStr">
-        <is>
-          <t>2020-05-10</t>
-        </is>
-      </c>
-      <c r="B112" t="n">
-        <v>1336478</v>
-      </c>
-      <c r="C112" t="n">
-        <v>79765</v>
-      </c>
-      <c r="D112" t="inlineStr">
-        <is>
-          <t>Sunday</t>
-        </is>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="inlineStr">
-        <is>
-          <t>2020-05-11</t>
-        </is>
-      </c>
-      <c r="B113" t="n">
-        <v>1354096</v>
-      </c>
-      <c r="C113" t="n">
-        <v>80747</v>
-      </c>
-      <c r="D113" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="inlineStr">
-        <is>
-          <t>2020-05-12</t>
-        </is>
-      </c>
-      <c r="B114" t="n">
-        <v>1376388</v>
-      </c>
-      <c r="C114" t="n">
-        <v>82402</v>
-      </c>
-      <c r="D114" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" t="inlineStr">
-        <is>
-          <t>2020-05-13</t>
-        </is>
-      </c>
-      <c r="B115" t="n">
-        <v>1397520</v>
-      </c>
-      <c r="C115" t="n">
-        <v>84170</v>
-      </c>
-      <c r="D115" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" t="inlineStr">
-        <is>
-          <t>2020-05-14</t>
-        </is>
-      </c>
-      <c r="B116" t="n">
-        <v>1424474</v>
-      </c>
-      <c r="C116" t="n">
-        <v>85908</v>
-      </c>
-      <c r="D116" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" t="inlineStr">
-        <is>
-          <t>2020-05-15</t>
-        </is>
-      </c>
-      <c r="B117" t="n">
-        <v>1450700</v>
-      </c>
-      <c r="C117" t="n">
-        <v>87501</v>
-      </c>
-      <c r="D117" t="inlineStr">
-        <is>
           <t>Friday</t>
         </is>
       </c>
-    </row>
-    <row r="118">
-      <c r="A118" t="inlineStr">
-        <is>
-          <t>2020-05-16</t>
-        </is>
-      </c>
-      <c r="B118" t="n">
-        <v>1474351</v>
-      </c>
-      <c r="C118" t="n">
-        <v>88726</v>
-      </c>
-      <c r="D118" t="inlineStr">
-        <is>
-          <t>Saturday</t>
-        </is>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" t="inlineStr">
-        <is>
-          <t>2020-05-17</t>
-        </is>
-      </c>
-      <c r="B119" t="n">
-        <v>1493350</v>
-      </c>
-      <c r="C119" t="n">
-        <v>89570</v>
-      </c>
-      <c r="D119" t="inlineStr">
-        <is>
-          <t>Sunday</t>
-        </is>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" t="inlineStr">
-        <is>
-          <t>2020-05-18</t>
-        </is>
-      </c>
-      <c r="B120" t="n">
-        <v>1515177</v>
-      </c>
-      <c r="C120" t="n">
-        <v>90416</v>
-      </c>
-      <c r="D120" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" t="inlineStr">
-        <is>
-          <t>2020-05-19</t>
-        </is>
-      </c>
-      <c r="B121" t="n">
-        <v>1536129</v>
-      </c>
-      <c r="C121" t="n">
-        <v>91936</v>
-      </c>
-      <c r="D121" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" t="inlineStr">
-        <is>
-          <t>2020-05-20</t>
-        </is>
-      </c>
-      <c r="B122" t="n">
-        <v>1559003</v>
-      </c>
-      <c r="C122" t="n">
-        <v>93408</v>
-      </c>
-      <c r="D122" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" t="inlineStr">
-        <is>
-          <t>2020-05-21</t>
-        </is>
-      </c>
-      <c r="B123" t="n">
-        <v>1584826</v>
-      </c>
-      <c r="C123" t="n">
-        <v>94722</v>
-      </c>
-      <c r="D123" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" t="inlineStr">
-        <is>
-          <t>2020-05-22</t>
-        </is>
-      </c>
-      <c r="B124" t="n">
-        <v>1608710</v>
-      </c>
-      <c r="C124" t="n">
-        <v>96011</v>
-      </c>
-      <c r="D124" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
+      <c r="E111" t="n">
+        <v>24566</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Newer data and Abstract completed in Paper
</commit_message>
<xml_diff>
--- a/excel_files/US.xlsx
+++ b/excel_files/US.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E111"/>
+  <dimension ref="A1:E112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2703,6 +2703,27 @@
         <v>24566</v>
       </c>
     </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>2020-05-30</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
+        <v>1778017</v>
+      </c>
+      <c r="C112" t="n">
+        <v>103775</v>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>Saturday</t>
+        </is>
+      </c>
+      <c r="E112" t="n">
+        <v>23293</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>